<commit_message>
Post SIT Cybersource OCBC|MDR, Cybersource Paymaya & Update functional Molpay SGD
</commit_message>
<xml_diff>
--- a/Traveloka_DataAutomation_Portal_Molpaysgd/Data/Config.xlsx
+++ b/Traveloka_DataAutomation_Portal_Molpaysgd/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\Traveloka_DataAutomation_Portal_Molpaysgd\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA9D823-4457-4F45-AB15-CB152686C647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC525F9-4ED0-4AC4-ACE1-F8CF8D43812D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="71">
   <si>
     <t>Name</t>
   </si>
@@ -240,6 +240,12 @@
   </si>
   <si>
     <t>RPA044_MOLPAY_Captcha_SiteKey</t>
+  </si>
+  <si>
+    <t>TemplateMolpayFee</t>
+  </si>
+  <si>
+    <t>C:\Kalyana\Traveloka_DataAutomation_Portal_Molpaysgd\Data\Template\Molpay Fee.xlsx</t>
   </si>
 </sst>
 </file>
@@ -618,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="14.95" customHeight="1"/>
@@ -713,7 +719,14 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.3" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.3" customHeight="1">
+      <c r="A8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" t="s">
+        <v>70</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.3" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.3" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.3" customHeight="1"/>
@@ -2876,8 +2889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="14.95" customHeight="1"/>

</xml_diff>

<commit_message>
Update Molpay SGD config prod & Molpay SGD Fee selector download report to hardware click
</commit_message>
<xml_diff>
--- a/Traveloka_DataAutomation_Portal_Molpaysgd/Data/Config.xlsx
+++ b/Traveloka_DataAutomation_Portal_Molpaysgd/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\dataautomation_personal\Traveloka_DataAutomation_Portal_Molpaysgd\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FA7C36-0A67-4D17-A387-58DE59FFEB76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD82F16-6FF6-4A27-8915-97857B0B15D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11508" windowHeight="11280" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3552" yWindow="3552" windowWidth="21588" windowHeight="10620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -197,9 +197,6 @@
     <t>MerchantId</t>
   </si>
   <si>
-    <t>[Dev] RPA_Moon_UploadBucket</t>
-  </si>
-  <si>
     <t>OrchestratorQueueName</t>
   </si>
   <si>
@@ -221,9 +218,6 @@
     <t>TemplateMolpayFee</t>
   </si>
   <si>
-    <t>C:\Kalyana\Traveloka_DataAutomation_Portal_Molpaysgd\Data\Template\Molpay Fee.xlsx</t>
-  </si>
-  <si>
     <t>RPA_Moon_SheetIdConfig</t>
   </si>
   <si>
@@ -246,6 +240,12 @@
   </si>
   <si>
     <t>RPA044_MOLPAY_SG_Captcha_RuleId</t>
+  </si>
+  <si>
+    <t>RPA_Moon_UploadBucket</t>
+  </si>
+  <si>
+    <t>Data\Template\Molpay Fee.xlsx</t>
   </si>
 </sst>
 </file>
@@ -624,7 +624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -672,10 +672,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.3" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -721,10 +721,10 @@
     </row>
     <row r="8" spans="1:26" ht="14.3" customHeight="1">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.3" customHeight="1"/>
@@ -2889,7 +2889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6:B8"/>
     </sheetView>
   </sheetViews>
@@ -2942,7 +2942,7 @@
         <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.3" customHeight="1">
@@ -2950,7 +2950,7 @@
         <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.3" customHeight="1">
@@ -2958,7 +2958,7 @@
         <v>46</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.3" customHeight="1">
@@ -2966,7 +2966,7 @@
         <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.3" customHeight="1">
@@ -2974,7 +2974,7 @@
         <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.3" customHeight="1">
@@ -2982,7 +2982,7 @@
         <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.3" customHeight="1">
@@ -2990,31 +2990,31 @@
         <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.3" customHeight="1">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.3" customHeight="1">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.3" customHeight="1">
       <c r="A11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" t="s">
         <v>58</v>
-      </c>
-      <c r="B11" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.3" customHeight="1"/>

</xml_diff>

<commit_message>
Pending update molpaysgd & molpaysgdfee
</commit_message>
<xml_diff>
--- a/Traveloka_DataAutomation_Portal_Molpaysgd/Data/Config.xlsx
+++ b/Traveloka_DataAutomation_Portal_Molpaysgd/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\dataautomation_personal\Traveloka_DataAutomation_Portal_Molpaysgd\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01401163-93FA-42B4-A500-B27A640222BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD82F16-6FF6-4A27-8915-97857B0B15D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="1680" windowWidth="17268" windowHeight="8196" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3552" yWindow="3552" windowWidth="21588" windowHeight="10620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -197,9 +197,6 @@
     <t>MerchantId</t>
   </si>
   <si>
-    <t>[Dev] RPA_Moon_UploadBucket</t>
-  </si>
-  <si>
     <t>OrchestratorQueueName</t>
   </si>
   <si>
@@ -209,24 +206,6 @@
     <t>DialogDownloadChrome</t>
   </si>
   <si>
-    <t>[Dev] RPA_Moon_SheetIdConfig</t>
-  </si>
-  <si>
-    <t>[Dev] RPA_Moon_PathMasterFolder</t>
-  </si>
-  <si>
-    <t>[Dev] RPA_Moon_PathMailTemplate</t>
-  </si>
-  <si>
-    <t>[Dev] RPA_Moon_PathSaKey</t>
-  </si>
-  <si>
-    <t>[Dev] RPA_Moon_PathDownloadChrome</t>
-  </si>
-  <si>
-    <t>[Dev] RPA_Moon_DialogDownloadChrome</t>
-  </si>
-  <si>
     <t>SenderName</t>
   </si>
   <si>
@@ -239,13 +218,34 @@
     <t>TemplateMolpayFee</t>
   </si>
   <si>
-    <t>C:\Kalyana\Traveloka_DataAutomation_Portal_Molpaysgd\Data\Template\Molpay Fee.xlsx</t>
+    <t>RPA_Moon_SheetIdConfig</t>
+  </si>
+  <si>
+    <t>RPA_Moon_PathMasterFolder</t>
+  </si>
+  <si>
+    <t>RPA_Moon_PathMailTemplate</t>
+  </si>
+  <si>
+    <t>RPA_Moon_PathSaKey</t>
+  </si>
+  <si>
+    <t>RPA_Moon_PathDownloadChrome</t>
+  </si>
+  <si>
+    <t>RPA_Moon_DialogDownloadChrome</t>
+  </si>
+  <si>
+    <t>RPA044_MOLPAY_SG_Captcha_SiteKey</t>
   </si>
   <si>
     <t>RPA044_MOLPAY_SG_Captcha_RuleId</t>
   </si>
   <si>
-    <t>RPA044_MOLPAY_SG_Captcha_SiteKey</t>
+    <t>RPA_Moon_UploadBucket</t>
+  </si>
+  <si>
+    <t>Data\Template\Molpay Fee.xlsx</t>
   </si>
 </sst>
 </file>
@@ -624,7 +624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -672,10 +672,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.3" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -721,10 +721,10 @@
     </row>
     <row r="8" spans="1:26" ht="14.3" customHeight="1">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.3" customHeight="1"/>
@@ -2889,8 +2889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="14.95" customHeight="1"/>
@@ -2942,7 +2942,7 @@
         <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.3" customHeight="1">
@@ -2950,7 +2950,7 @@
         <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.3" customHeight="1">
@@ -2958,7 +2958,7 @@
         <v>46</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.3" customHeight="1">
@@ -2966,7 +2966,7 @@
         <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.3" customHeight="1">
@@ -2974,7 +2974,7 @@
         <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.3" customHeight="1">
@@ -2982,7 +2982,7 @@
         <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.3" customHeight="1">
@@ -2990,31 +2990,31 @@
         <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.3" customHeight="1">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.3" customHeight="1">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.3" customHeight="1">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.3" customHeight="1"/>

</xml_diff>